<commit_message>
Moving and tidy-up of Shiny app code
</commit_message>
<xml_diff>
--- a/data/Open Budget category for model.xlsx
+++ b/data/Open Budget category for model.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0f4a93aa42a454b8/Рабочий стол/Bank/ob_28_10/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrii/Documents/R files/_My projects/Open budget/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{ED482BD7-F917-4704-859C-F87943722102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AE8FC548-BC76-4304-9B4E-DBAECDD84D19}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87D06D66-A20A-D64A-8D99-1FA1EB8E86CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{1ACCA768-2D17-4B0E-9B17-CEC269EEEDB6}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="16760" windowHeight="15000" xr2:uid="{1ACCA768-2D17-4B0E-9B17-CEC269EEEDB6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
@@ -496,16 +496,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7459D5F-A6DE-4359-9231-3041E2ABD2A2}">
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="57" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="15.1796875" customWidth="1"/>
+    <col min="2" max="2" width="41" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -519,7 +521,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -533,7 +535,7 @@
         <v>2199</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -547,7 +549,7 @@
         <v>2249</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -561,7 +563,7 @@
         <v>2269</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -575,7 +577,7 @@
         <v>2279</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -589,7 +591,7 @@
         <v>2281</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -603,7 +605,7 @@
         <v>2399</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -617,7 +619,7 @@
         <v>2599</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -631,7 +633,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -645,7 +647,7 @@
         <v>2699</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -659,7 +661,7 @@
         <v>2799</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -673,7 +675,7 @@
         <v>2999</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -687,7 +689,7 @@
         <v>3199</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -701,7 +703,7 @@
         <v>3219</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -715,7 +717,7 @@
         <v>8999</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -729,7 +731,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -743,7 +745,7 @@
         <v>11019999</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -757,7 +759,7 @@
         <v>13999999</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -771,7 +773,7 @@
         <v>14999999</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -785,7 +787,7 @@
         <v>18049999</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>15</v>
       </c>
@@ -799,7 +801,7 @@
         <v>18059999</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>15</v>
       </c>
@@ -813,7 +815,7 @@
         <v>19999999</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>15</v>
       </c>
@@ -827,7 +829,7 @@
         <v>21010499</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>15</v>
       </c>
@@ -841,7 +843,7 @@
         <v>21010599</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>15</v>
       </c>
@@ -855,7 +857,7 @@
         <v>21010699</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>15</v>
       </c>
@@ -869,7 +871,7 @@
         <v>21011199</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>15</v>
       </c>
@@ -883,7 +885,7 @@
         <v>24109999</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>15</v>
       </c>
@@ -897,7 +899,7 @@
         <v>24119999</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>15</v>
       </c>
@@ -911,7 +913,7 @@
         <v>29999999</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>15</v>
       </c>
@@ -925,7 +927,7 @@
         <v>39999999</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>15</v>
       </c>
@@ -939,7 +941,7 @@
         <v>41999999</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>15</v>
       </c>
@@ -953,7 +955,7 @@
         <v>42999999</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>15</v>
       </c>
@@ -967,7 +969,7 @@
         <v>49999999</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
the transfers adjustment included in monitoring table
</commit_message>
<xml_diff>
--- a/data/Open Budget category for model.xlsx
+++ b/data/Open Budget category for model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0f4a93aa42a454b8/Рабочий стол/Bank/ob_22_11_23/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{87D06D66-A20A-D64A-8D99-1FA1EB8E86CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AB83B83C-D884-4647-9734-67E3923E2133}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{87D06D66-A20A-D64A-8D99-1FA1EB8E86CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{767500F2-7C76-4BB0-83DC-6C3A920A932F}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{1ACCA768-2D17-4B0E-9B17-CEC269EEEDB6}"/>
   </bookViews>
@@ -180,10 +180,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -501,7 +500,7 @@
   <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C28" sqref="A28:XFD29"/>
+      <selection activeCell="C28" sqref="C28:D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -889,31 +888,31 @@
         <v>21049999</v>
       </c>
     </row>
-    <row r="28" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B28" s="2" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" t="s">
         <v>21</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28">
         <v>21050000</v>
       </c>
-      <c r="D28" s="2">
-        <v>21059999</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B29" s="2" t="s">
+      <c r="D28">
+        <v>21050001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29" t="s">
         <v>26</v>
       </c>
-      <c r="C29" s="2">
-        <v>21060000</v>
-      </c>
-      <c r="D29" s="2">
+      <c r="C29">
+        <v>21050002</v>
+      </c>
+      <c r="D29">
         <v>24109999</v>
       </c>
     </row>

</xml_diff>